<commit_message>
chore: Refactor e2e test kindliste
</commit_message>
<xml_diff>
--- a/e2e_tests/test_uploads/Kindliste.xlsx
+++ b/e2e_tests/test_uploads/Kindliste.xlsx
@@ -31,12 +31,12 @@
     <t xml:space="preserve">Geburtsdatum</t>
   </si>
   <si>
+    <t xml:space="preserve">Aufnahmedatum</t>
+  </si>
+  <si>
     <t xml:space="preserve">Entlassungsdatum</t>
   </si>
   <si>
-    <t xml:space="preserve">Aufnahmedatum</t>
-  </si>
-  <si>
     <t xml:space="preserve">Anna</t>
   </si>
   <si>
@@ -46,24 +46,24 @@
     <t xml:space="preserve">18.11.2022</t>
   </si>
   <si>
+    <t xml:space="preserve">18.11.2023</t>
+  </si>
+  <si>
     <t xml:space="preserve">31.07.2029</t>
   </si>
   <si>
-    <t xml:space="preserve">18.11.2023</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mohammed</t>
   </si>
   <si>
     <t xml:space="preserve">10.11.2020</t>
   </si>
   <si>
+    <t xml:space="preserve">10.11.2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">31.07.2027</t>
   </si>
   <si>
-    <t xml:space="preserve">10.11.2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bilbo</t>
   </si>
   <si>
@@ -94,12 +94,12 @@
     <t xml:space="preserve">10.10.2023</t>
   </si>
   <si>
+    <t xml:space="preserve">10.10.2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">31.07.2030</t>
   </si>
   <si>
-    <t xml:space="preserve">10.10.2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pippin</t>
   </si>
   <si>
@@ -121,10 +121,10 @@
     <t xml:space="preserve">08.05.2022</t>
   </si>
   <si>
+    <t xml:space="preserve">08.05.2024</t>
+  </si>
+  <si>
     <t xml:space="preserve">31.07.2028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08.05.2024</t>
   </si>
   <si>
     <t xml:space="preserve">Fredegar</t>
@@ -524,20 +524,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="3" width="18.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="3" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="18.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="18.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="3" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,7 +558,7 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -574,7 +576,7 @@
       <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -592,7 +594,7 @@
       <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -605,12 +607,12 @@
         <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -623,12 +625,12 @@
         <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
@@ -646,7 +648,7 @@
       <c r="E6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -659,12 +661,12 @@
         <v>28</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
@@ -682,7 +684,7 @@
       <c r="E8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
@@ -695,12 +697,12 @@
         <v>37</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
@@ -713,12 +715,12 @@
         <v>41</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
@@ -731,12 +733,12 @@
         <v>45</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
@@ -749,12 +751,12 @@
         <v>48</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
@@ -767,12 +769,12 @@
         <v>52</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -785,12 +787,12 @@
         <v>56</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
@@ -803,12 +805,12 @@
         <v>60</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="G15" s="5"/>
     </row>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>